<commit_message>
Remove CODPlayerDetectionDataset from .gitignore; add session_data.csv and multiple label files for training and validation
</commit_message>
<xml_diff>
--- a/cnn_data.xlsx
+++ b/cnn_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,7 +459,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -467,7 +467,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -502,7 +502,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -510,7 +510,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" t="b">
         <v>0</v>
@@ -531,7 +531,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" t="b">
         <v>0</v>
@@ -550,7 +550,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -558,7 +558,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -587,7 +587,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" t="b">
         <v>0</v>
@@ -595,15 +595,15 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
@@ -614,7 +614,7 @@
         <v>20</v>
       </c>
       <c r="B24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -630,6 +630,254 @@
         <v>22</v>
       </c>
       <c r="B26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>23</v>
+      </c>
+      <c r="B27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>24</v>
+      </c>
+      <c r="B28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>25</v>
+      </c>
+      <c r="B29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>26</v>
+      </c>
+      <c r="B30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>26</v>
+      </c>
+      <c r="B31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>27</v>
+      </c>
+      <c r="B32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>28</v>
+      </c>
+      <c r="B33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>29</v>
+      </c>
+      <c r="B34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>30</v>
+      </c>
+      <c r="B35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>31</v>
+      </c>
+      <c r="B36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32</v>
+      </c>
+      <c r="B37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>33</v>
+      </c>
+      <c r="B38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>33</v>
+      </c>
+      <c r="B39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>34</v>
+      </c>
+      <c r="B40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>35</v>
+      </c>
+      <c r="B41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>36</v>
+      </c>
+      <c r="B42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>37</v>
+      </c>
+      <c r="B43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>38</v>
+      </c>
+      <c r="B44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>39</v>
+      </c>
+      <c r="B45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>40</v>
+      </c>
+      <c r="B46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>41</v>
+      </c>
+      <c r="B47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>41</v>
+      </c>
+      <c r="B48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>42</v>
+      </c>
+      <c r="B49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>43</v>
+      </c>
+      <c r="B50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>44</v>
+      </c>
+      <c r="B51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>45</v>
+      </c>
+      <c r="B52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>46</v>
+      </c>
+      <c r="B53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>47</v>
+      </c>
+      <c r="B54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>48</v>
+      </c>
+      <c r="B55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>48</v>
+      </c>
+      <c r="B56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>49</v>
+      </c>
+      <c r="B57" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update session data and enhance model training; modify launch script for new data handling and improve GUI elements
</commit_message>
<xml_diff>
--- a/cnn_data.xlsx
+++ b/cnn_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,7 +435,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -443,7 +443,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
@@ -459,7 +459,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -467,7 +467,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -475,7 +475,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
@@ -483,7 +483,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
@@ -499,31 +499,31 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B13" t="b">
         <v>0</v>
@@ -531,15 +531,15 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B15" t="b">
         <v>0</v>
@@ -547,15 +547,15 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B18" t="b">
         <v>0</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" t="b">
         <v>0</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20" t="b">
         <v>0</v>
@@ -587,15 +587,15 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B22" t="b">
         <v>0</v>
@@ -603,23 +603,23 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B25" t="b">
         <v>0</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
@@ -643,15 +643,15 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B29" t="b">
         <v>0</v>
@@ -659,7 +659,7 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
@@ -667,7 +667,7 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B31" t="b">
         <v>0</v>
@@ -675,7 +675,7 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B32" t="b">
         <v>0</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B34" t="b">
         <v>0</v>
@@ -699,15 +699,15 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B36" t="b">
         <v>0</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B37" t="b">
         <v>0</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B38" t="b">
         <v>0</v>
@@ -731,7 +731,7 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B39" t="b">
         <v>0</v>
@@ -739,7 +739,7 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B40" t="b">
         <v>0</v>
@@ -747,7 +747,7 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B41" t="b">
         <v>0</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B42" t="b">
         <v>0</v>
@@ -763,7 +763,7 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B43" t="b">
         <v>0</v>
@@ -771,7 +771,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B44" t="b">
         <v>0</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B45" t="b">
         <v>0</v>
@@ -787,15 +787,15 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B47" t="b">
         <v>1</v>
@@ -803,7 +803,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B48" t="b">
         <v>0</v>
@@ -811,7 +811,7 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B49" t="b">
         <v>0</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B50" t="b">
         <v>0</v>
@@ -827,15 +827,15 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B52" t="b">
         <v>0</v>
@@ -843,7 +843,7 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B53" t="b">
         <v>0</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B54" t="b">
         <v>0</v>
@@ -859,7 +859,7 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B55" t="b">
         <v>0</v>
@@ -867,17 +867,201 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>52</v>
+      </c>
+      <c r="B58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>53</v>
+      </c>
+      <c r="B59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>54</v>
+      </c>
+      <c r="B60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>55</v>
+      </c>
+      <c r="B61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>56</v>
+      </c>
+      <c r="B62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>57</v>
+      </c>
+      <c r="B63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>58</v>
+      </c>
+      <c r="B64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>58</v>
+      </c>
+      <c r="B65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>59</v>
+      </c>
+      <c r="B66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>60</v>
+      </c>
+      <c r="B67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>61</v>
+      </c>
+      <c r="B68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>62</v>
+      </c>
+      <c r="B69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>63</v>
+      </c>
+      <c r="B70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>64</v>
+      </c>
+      <c r="B71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>65</v>
+      </c>
+      <c r="B72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>65</v>
+      </c>
+      <c r="B73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>66</v>
+      </c>
+      <c r="B74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>67</v>
+      </c>
+      <c r="B75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>68</v>
+      </c>
+      <c r="B76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>69</v>
+      </c>
+      <c r="B77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>70</v>
+      </c>
+      <c r="B78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>71</v>
+      </c>
+      <c r="B79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>71</v>
+      </c>
+      <c r="B80" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>